<commit_message>
update mortality and morbidity
</commit_message>
<xml_diff>
--- a/output/Tables/HIA_per_disease.xlsx
+++ b/output/Tables/HIA_per_disease.xlsx
@@ -1,21 +1,137 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ines/Documents/M2/ENS/Stage/Walking benefits/codes/walking/output/Tables/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7832F83-F290-AB4B-83B8-F90F96AF2649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+  <si>
+    <t>disease</t>
+  </si>
+  <si>
+    <t>tot_cases</t>
+  </si>
+  <si>
+    <t>tot_daly</t>
+  </si>
+  <si>
+    <t>tot_medic_costs</t>
+  </si>
+  <si>
+    <t>tot_soc_costs</t>
+  </si>
+  <si>
+    <t>cc</t>
+  </si>
+  <si>
+    <t>1258.913 (524.192 - 1976.014)</t>
+  </si>
+  <si>
+    <t>1353.242 (667.676 - 2121.708)</t>
+  </si>
+  <si>
+    <t>33.719 (14.394 - 53.164)</t>
+  </si>
+  <si>
+    <t>180.104 (90.023 - 283.337)</t>
+  </si>
+  <si>
+    <t>dem</t>
+  </si>
+  <si>
+    <t>1968.05 (890.542 - 2989.415)</t>
+  </si>
+  <si>
+    <t>1648.83 (749.536 - 2494.483)</t>
+  </si>
+  <si>
+    <t>44.736 (20.329 - 68.022)</t>
+  </si>
+  <si>
+    <t>218.917 (99.63 - 332.089)</t>
+  </si>
+  <si>
+    <t>bc</t>
+  </si>
+  <si>
+    <t>4366.409 (2302.003 - 6892.274)</t>
+  </si>
+  <si>
+    <t>6819.038 (3576.478 - 10865.739)</t>
+  </si>
+  <si>
+    <t>205.132 (109.061 - 324.53)</t>
+  </si>
+  <si>
+    <t>905.949 (477.481 - 1435.349)</t>
+  </si>
+  <si>
+    <t>cvd</t>
+  </si>
+  <si>
+    <t>14551.942 (9087.139 - 22082.782)</t>
+  </si>
+  <si>
+    <t>10145.346 (6361.807 - 15350.398)</t>
+  </si>
+  <si>
+    <t>305.844 (189.099 - 463.339)</t>
+  </si>
+  <si>
+    <t>1350.491 (844.968 - 2042.131)</t>
+  </si>
+  <si>
+    <t>diab2</t>
+  </si>
+  <si>
+    <t>19293.832 (10137.691 - 30176.726)</t>
+  </si>
+  <si>
+    <t>26426.126 (13717.799 - 41756.946)</t>
+  </si>
+  <si>
+    <t>706.314 (366.723 - 1099.463)</t>
+  </si>
+  <si>
+    <t>3516.705 (1833.915 - 5498.078)</t>
+  </si>
+  <si>
+    <t>mort</t>
+  </si>
+  <si>
+    <t>17842.225 (7314.864 - 28025.149)</t>
+  </si>
+  <si>
+    <t>172174.881 (70655.009 - 271634.011)</t>
+  </si>
+  <si>
+    <t>0 (0 - 0)</t>
+  </si>
+  <si>
+    <t>22919.746 (9292.411 - 36318.5)</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,13 +179,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -107,7 +231,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -141,6 +265,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -175,9 +300,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -350,200 +476,137 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.83203125" customWidth="1"/>
+    <col min="2" max="5" width="31.33203125" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>disease</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>tot_cases</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>tot_daly</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>tot_medic_costs</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>tot_soc_costs</t>
-        </is>
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>cc</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>1258.913 (524.192 - 1976.014)</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>1353.242 (667.676 - 2121.708)</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>33.719 (14.394 - 53.164)</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>180.104 (90.023 - 283.337)</t>
-        </is>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>dem</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>1968.05 (890.542 - 2989.415)</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>1648.83 (749.536 - 2494.483)</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>44.736 (20.329 - 68.022)</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>218.917 (99.63 - 332.089)</t>
-        </is>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>bc</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>4366.409 (2302.003 - 6892.274)</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>6819.038 (3576.478 - 10865.739)</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>205.132 (109.061 - 324.53)</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>905.949 (477.481 - 1435.349)</t>
-        </is>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>cvd</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>14551.942 (9087.139 - 22082.782)</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>10145.346 (6361.807 - 15350.398)</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>305.844 (189.099 - 463.339)</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>1350.491 (844.968 - 2042.131)</t>
-        </is>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>diab2</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>19293.832 (10137.691 - 30176.726)</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>26426.126 (13717.799 - 41756.946)</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>706.314 (366.723 - 1099.463)</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>3516.705 (1833.915 - 5498.078)</t>
-        </is>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>mort</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>17842.225 (7314.864 - 28025.149)</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>172174.881 (70655.009 - 271634.011)</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>0 (0 - 0)</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>22919.746 (9292.411 - 36318.5)</t>
-        </is>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>